<commit_message>
TF IDF results added
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>News data results</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>After removing stopwords/stemming/lemmatization</t>
+  </si>
+  <si>
+    <t>TF-IDF</t>
+  </si>
+  <si>
+    <t>k=5: 0.6349206349206349</t>
+  </si>
+  <si>
+    <t>k=10: 0.6031746031746031</t>
+  </si>
+  <si>
+    <t>k=30: 0.5608465608465608</t>
+  </si>
+  <si>
+    <t>k=40: 0.49206349206349204</t>
   </si>
 </sst>
 </file>
@@ -181,7 +196,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,8 +227,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -301,11 +328,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -330,16 +372,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -643,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,15 +960,15 @@
       <c r="G15" s="7">
         <v>0.79100529100529104</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="16">
         <v>0.87566137566137503</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="17">
         <v>0.85978835978835899</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -927,7 +980,7 @@
       <c r="D16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -941,7 +994,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -951,7 +1004,7 @@
       <c r="D17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="5" t="s">
         <v>35</v>
       </c>
@@ -963,7 +1016,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -973,7 +1026,7 @@
       <c r="D18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="5" t="s">
         <v>36</v>
       </c>
@@ -985,7 +1038,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
@@ -995,7 +1048,7 @@
       <c r="D19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="5" t="s">
         <v>19</v>
       </c>
@@ -1007,7 +1060,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="10" t="s">
         <v>20</v>
       </c>
@@ -1017,7 +1070,7 @@
       <c r="D20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="17"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="10" t="s">
         <v>20</v>
       </c>
@@ -1028,13 +1081,97 @@
         <v>41</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="21"/>
+    </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="15"/>
+      <c r="A23" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="22">
+        <v>0.83862433862433805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="22">
+        <v>0.81481481481481399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="22">
+        <v>0.68518518518518501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="24">
+        <v>0.84656084656084596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="22">
+        <v>0.58994708994709</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="22">
+        <v>0.79365079365079305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="F16:F20"/>
+    <mergeCell ref="A29:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>